<commit_message>
redone so the graphs are still ineractactble
</commit_message>
<xml_diff>
--- a/output/sample2_results.xlsx
+++ b/output/sample2_results.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="ROC_Data" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="63">
   <si>
     <t>Compound</t>
   </si>
@@ -180,6 +181,30 @@
   </si>
   <si>
     <t>01_Blank_1</t>
+  </si>
+  <si>
+    <t>FPR_G_All</t>
+  </si>
+  <si>
+    <t>TPR_G_All</t>
+  </si>
+  <si>
+    <t>FPR_F_All</t>
+  </si>
+  <si>
+    <t>TPR_F_All</t>
+  </si>
+  <si>
+    <t>FPR_G_NB</t>
+  </si>
+  <si>
+    <t>TPR_G_NB</t>
+  </si>
+  <si>
+    <t>FPR_F_NB</t>
+  </si>
+  <si>
+    <t>TPR_F_NB</t>
   </si>
 </sst>
 </file>
@@ -252,9 +277,633 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ROC (with blanks)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Compound G</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ROC_Data!$A$2:$A$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.09090909090909091</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.09090909090909091</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.4545454545454545</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.5454545454545454</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.5454545454545454</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ROC_Data!$B$2:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05263157894736842</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.1842105263157895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2894736842105263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.3684210526315789</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6842105263157895</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8157894736842105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.8157894736842105</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.9473684210526315</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.9473684210526315</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.9473684210526315</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Compound F</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ROC_Data!$C$2:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.1666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.4166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5833333333333334</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ROC_Data!$D$2:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.07894736842105263</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2368421052631579</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.2894736842105263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.6842105263157895</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.7368421052631579</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8947368421052632</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.8947368421052632</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50010001"/>
+        <c:axId val="50010002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50010001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>False Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50010002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>True Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50010001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>ROC (non-blanks only)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Compound G</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="0000FF"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ROC_Data!$E$2:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.7142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ROC_Data!$F$2:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.06451612903225806</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2258064516129032</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3548387096774194</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.4516129032258064</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.6129032258064516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.8387096774193549</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Compound F</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>ROC_Data!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>ROC_Data!$H$2:$H$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.08823529411764706</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.2647058823529412</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.3235294117647059</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.7647058823529411</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8235294117647058</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="50020001"/>
+        <c:axId val="50020002"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="50020001"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>False Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020002"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="50020002"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>True Positive Rate</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="50020001"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -262,37 +911,29 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>365772</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>7629</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="sample2_results_roc_with_blanks.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315200" y="190500"/>
-          <a:ext cx="5852172" cy="4389129"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>0</xdr:colOff>
@@ -300,34 +941,26 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>365772</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>7629</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="sample2_results_roc_non_blanks.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7315200" y="3619500"/>
-          <a:ext cx="5852172" cy="4389129"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -1666,4 +2299,335 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0.07894736842105263</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.06451612903225806</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0.08823529411764706</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0.1842105263157895</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0.2368421052631579</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.2258064516129032</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.2647058823529412</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0.2894736842105263</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0.2894736842105263</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.3548387096774194</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0.3235294117647059</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0.3684210526315789</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0.6842105263157895</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.4516129032258064</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0.7647058823529411</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0.5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.6129032258064516</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.8235294117647058</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0.6842105263157895</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0.8947368421052632</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.8387096774193549</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0.8157894736842105</v>
+      </c>
+      <c r="C9">
+        <v>0.1666666666666667</v>
+      </c>
+      <c r="D9">
+        <v>0.8947368421052632</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="B10">
+        <v>0.8157894736842105</v>
+      </c>
+      <c r="C10">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="B11">
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="C11">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="B12">
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="C12">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>0.5454545454545454</v>
+      </c>
+      <c r="B13">
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>0.5454545454545454</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>